<commit_message>
fix spelling of definition
</commit_message>
<xml_diff>
--- a/data/outlookClasses.xlsx
+++ b/data/outlookClasses.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FINNISS\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FINNISS\Desktop\salmonOutlookReportCode\salmon-outlook-report\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C72D1F0-4990-447B-8040-91C29A5A3024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8453BC-C76B-4FFD-8F92-F7AD48E1E4C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{BB8E1D3B-B39C-4B8D-B424-5EE9BE023372}"/>
   </bookViews>
@@ -53,9 +53,6 @@
     <t>Precautionary Approach (SMU  Level)</t>
   </si>
   <si>
-    <t>Category Definitino</t>
-  </si>
-  <si>
     <t>Expected spawning abundance</t>
   </si>
   <si>
@@ -198,6 +195,9 @@
   </si>
   <si>
     <t>Green Zone (i.e., at or above the TRP)</t>
+  </si>
+  <si>
+    <t>Category Definition</t>
   </si>
 </sst>
 </file>
@@ -675,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E7470E5-2096-4511-8B0D-0EAB2F509ED4}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -712,10 +712,10 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="70.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -723,16 +723,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="112.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -740,16 +740,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>22</v>
-      </c>
       <c r="D4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="84.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -757,16 +757,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>24</v>
-      </c>
       <c r="D5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>11</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="56.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -774,29 +774,29 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="56.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>17</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add n/a in blank cells
</commit_message>
<xml_diff>
--- a/data/outlookClasses.xlsx
+++ b/data/outlookClasses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FINNISS\Desktop\salmonOutlookReportCode\salmon-outlook-report\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8453BC-C76B-4FFD-8F92-F7AD48E1E4C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B764A6A8-758A-46CF-B13F-DEE1172F34F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{BB8E1D3B-B39C-4B8D-B424-5EE9BE023372}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>Outlook Category</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>Category Definition</t>
+  </si>
+  <si>
+    <t>n/a</t>
   </si>
 </sst>
 </file>
@@ -675,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E7470E5-2096-4511-8B0D-0EAB2F509ED4}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -790,8 +793,12 @@
       <c r="A7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
+      <c r="B7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="D7" s="8" t="s">
         <v>16</v>
       </c>

</xml_diff>